<commit_message>
Converted Data Files to CSV
(Not tested)
</commit_message>
<xml_diff>
--- a/PROGRESS CHASE/Change Tracking.xlsx
+++ b/PROGRESS CHASE/Change Tracking.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\Github\Canada-CI\PROGRESS CHASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C06E64E-EB98-4663-9FE6-06D46A9C6CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CFA500-55CC-4E0E-B57D-5BA48032EFC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28058" windowHeight="16395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28058" windowHeight="16395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Improvements" sheetId="1" r:id="rId1"/>
     <sheet name="Debugging and Maintenance" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Tracking" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Check missing data for lower level NAICS codes in LFS. We need to modify the industry dimension to use higher level codes where the low-level codes are missing</t>
   </si>
@@ -69,6 +70,18 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>CSV files substituted for Dimension tables</t>
+  </si>
+  <si>
+    <t>Commit name</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>5a</t>
   </si>
 </sst>
 </file>
@@ -406,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B284C00-DDD4-47C6-B7FE-583F9746A79D}">
   <dimension ref="B3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -484,4 +497,38 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D800FF4-E029-4C77-B8C3-BD1498639AE5}">
+  <dimension ref="C2:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="45.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>